<commit_message>
Ingresos Egresos Muertes y Ingreso Raciones
</commit_message>
<xml_diff>
--- a/carga/mixer2.xlsx
+++ b/carga/mixer2.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgonzalez/.bitnami/stackman/machines/xampp/volumes/root/htdocs/feedlot/Archivos para Cargas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Dropbox\programa con Mauro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA35B4EF-C2DF-7F4F-AF95-612764FC924F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="DatosExternos_1" localSheetId="1" hidden="1">Hoja2!$A$1:$Y$54</definedName>
+    <definedName name="DatosExternos_1" localSheetId="1" hidden="1">Hoja2!$A$1:$Y$50</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,15 +28,15 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Consulta - PESADAS 15-10" description="Conexión a la consulta 'PESADAS 15-10' en el libro." type="5" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" keepAlive="1" name="Consulta - PESADAS 15-10" description="Conexión a la consulta 'PESADAS 15-10' en el libro." type="5" refreshedVersion="6" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=PESADAS 15-10;Extended Properties=&quot;&quot;" command="SELECT * FROM [PESADAS 15-10]"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="42">
   <si>
     <t>FECHA</t>
   </si>
@@ -164,14 +163,11 @@
   <si>
     <t xml:space="preserve">Lote 151        </t>
   </si>
-  <si>
-    <t>Lote 5</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
@@ -287,7 +283,7 @@
       <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -303,7 +299,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DatosExternos_1" connectionId="1" xr16:uid="{00000000-0016-0000-0100-000000000000}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatosExternos_1" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="26">
     <queryTableFields count="25">
       <queryTableField id="1" name="FECHA" tableColumnId="51"/>
@@ -337,34 +333,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="PESADAS_15_10" displayName="PESADAS_15_10" ref="A1:Y54" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:Y54" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="PESADAS_15_10" displayName="PESADAS_15_10" ref="A1:Y50" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:Y50"/>
   <tableColumns count="25">
-    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" uniqueName="51" name="FECHA" queryTableFieldId="1" dataDxfId="24"/>
-    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" uniqueName="52" name="HORA" queryTableFieldId="2" dataDxfId="23"/>
-    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" uniqueName="53" name="NUM" queryTableFieldId="3" dataDxfId="22"/>
-    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" uniqueName="54" name="DESCRIPCION" queryTableFieldId="4" dataDxfId="21"/>
-    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" uniqueName="55" name="ING_1" queryTableFieldId="5" dataDxfId="20"/>
-    <tableColumn id="56" xr3:uid="{00000000-0010-0000-0000-000038000000}" uniqueName="56" name="PESO_1" queryTableFieldId="6" dataDxfId="19"/>
-    <tableColumn id="57" xr3:uid="{00000000-0010-0000-0000-000039000000}" uniqueName="57" name="ING_2" queryTableFieldId="7" dataDxfId="18"/>
-    <tableColumn id="58" xr3:uid="{00000000-0010-0000-0000-00003A000000}" uniqueName="58" name="PESO_2" queryTableFieldId="8" dataDxfId="17"/>
-    <tableColumn id="59" xr3:uid="{00000000-0010-0000-0000-00003B000000}" uniqueName="59" name="ING_3" queryTableFieldId="9" dataDxfId="16"/>
-    <tableColumn id="60" xr3:uid="{00000000-0010-0000-0000-00003C000000}" uniqueName="60" name="PESO_3" queryTableFieldId="10" dataDxfId="15"/>
-    <tableColumn id="61" xr3:uid="{00000000-0010-0000-0000-00003D000000}" uniqueName="61" name="ING_4" queryTableFieldId="11" dataDxfId="14"/>
-    <tableColumn id="62" xr3:uid="{00000000-0010-0000-0000-00003E000000}" uniqueName="62" name="PESO_4" queryTableFieldId="12" dataDxfId="13"/>
-    <tableColumn id="63" xr3:uid="{00000000-0010-0000-0000-00003F000000}" uniqueName="63" name="ING_5" queryTableFieldId="13" dataDxfId="12"/>
-    <tableColumn id="64" xr3:uid="{00000000-0010-0000-0000-000040000000}" uniqueName="64" name="PESO_5" queryTableFieldId="14" dataDxfId="11"/>
-    <tableColumn id="65" xr3:uid="{00000000-0010-0000-0000-000041000000}" uniqueName="65" name="ING_6" queryTableFieldId="15" dataDxfId="10"/>
-    <tableColumn id="66" xr3:uid="{00000000-0010-0000-0000-000042000000}" uniqueName="66" name="PESO_6" queryTableFieldId="16" dataDxfId="9"/>
-    <tableColumn id="67" xr3:uid="{00000000-0010-0000-0000-000043000000}" uniqueName="67" name="ING_7" queryTableFieldId="17" dataDxfId="8"/>
-    <tableColumn id="68" xr3:uid="{00000000-0010-0000-0000-000044000000}" uniqueName="68" name="PESO_7" queryTableFieldId="18" dataDxfId="7"/>
-    <tableColumn id="69" xr3:uid="{00000000-0010-0000-0000-000045000000}" uniqueName="69" name="ING_8" queryTableFieldId="19" dataDxfId="6"/>
-    <tableColumn id="70" xr3:uid="{00000000-0010-0000-0000-000046000000}" uniqueName="70" name="PESO_8" queryTableFieldId="20" dataDxfId="5"/>
-    <tableColumn id="71" xr3:uid="{00000000-0010-0000-0000-000047000000}" uniqueName="71" name="ING_9" queryTableFieldId="21" dataDxfId="4"/>
-    <tableColumn id="72" xr3:uid="{00000000-0010-0000-0000-000048000000}" uniqueName="72" name="PESO_9" queryTableFieldId="22" dataDxfId="3"/>
-    <tableColumn id="73" xr3:uid="{00000000-0010-0000-0000-000049000000}" uniqueName="73" name="ING_10" queryTableFieldId="23" dataDxfId="2"/>
-    <tableColumn id="74" xr3:uid="{00000000-0010-0000-0000-00004A000000}" uniqueName="74" name="PESO_10" queryTableFieldId="24" dataDxfId="1"/>
-    <tableColumn id="75" xr3:uid="{00000000-0010-0000-0000-00004B000000}" uniqueName="75" name="TOTAL" queryTableFieldId="25" dataDxfId="0"/>
+    <tableColumn id="51" uniqueName="51" name="FECHA" queryTableFieldId="1" dataDxfId="24"/>
+    <tableColumn id="52" uniqueName="52" name="HORA" queryTableFieldId="2" dataDxfId="23"/>
+    <tableColumn id="53" uniqueName="53" name="NUM" queryTableFieldId="3" dataDxfId="22"/>
+    <tableColumn id="54" uniqueName="54" name="DESCRIPCION" queryTableFieldId="4" dataDxfId="21"/>
+    <tableColumn id="55" uniqueName="55" name="ING_1" queryTableFieldId="5" dataDxfId="20"/>
+    <tableColumn id="56" uniqueName="56" name="PESO_1" queryTableFieldId="6" dataDxfId="19"/>
+    <tableColumn id="57" uniqueName="57" name="ING_2" queryTableFieldId="7" dataDxfId="18"/>
+    <tableColumn id="58" uniqueName="58" name="PESO_2" queryTableFieldId="8" dataDxfId="17"/>
+    <tableColumn id="59" uniqueName="59" name="ING_3" queryTableFieldId="9" dataDxfId="16"/>
+    <tableColumn id="60" uniqueName="60" name="PESO_3" queryTableFieldId="10" dataDxfId="15"/>
+    <tableColumn id="61" uniqueName="61" name="ING_4" queryTableFieldId="11" dataDxfId="14"/>
+    <tableColumn id="62" uniqueName="62" name="PESO_4" queryTableFieldId="12" dataDxfId="13"/>
+    <tableColumn id="63" uniqueName="63" name="ING_5" queryTableFieldId="13" dataDxfId="12"/>
+    <tableColumn id="64" uniqueName="64" name="PESO_5" queryTableFieldId="14" dataDxfId="11"/>
+    <tableColumn id="65" uniqueName="65" name="ING_6" queryTableFieldId="15" dataDxfId="10"/>
+    <tableColumn id="66" uniqueName="66" name="PESO_6" queryTableFieldId="16" dataDxfId="9"/>
+    <tableColumn id="67" uniqueName="67" name="ING_7" queryTableFieldId="17" dataDxfId="8"/>
+    <tableColumn id="68" uniqueName="68" name="PESO_7" queryTableFieldId="18" dataDxfId="7"/>
+    <tableColumn id="69" uniqueName="69" name="ING_8" queryTableFieldId="19" dataDxfId="6"/>
+    <tableColumn id="70" uniqueName="70" name="PESO_8" queryTableFieldId="20" dataDxfId="5"/>
+    <tableColumn id="71" uniqueName="71" name="ING_9" queryTableFieldId="21" dataDxfId="4"/>
+    <tableColumn id="72" uniqueName="72" name="PESO_9" queryTableFieldId="22" dataDxfId="3"/>
+    <tableColumn id="73" uniqueName="73" name="ING_10" queryTableFieldId="23" dataDxfId="2"/>
+    <tableColumn id="74" uniqueName="74" name="PESO_10" queryTableFieldId="24" dataDxfId="1"/>
+    <tableColumn id="75" uniqueName="75" name="TOTAL" queryTableFieldId="25" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -632,55 +628,55 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Y54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -757,7 +753,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>43997</v>
       </c>
@@ -834,7 +830,7 @@
         <v>5750</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>43997</v>
       </c>
@@ -911,12 +907,12 @@
         <v>5890</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>43997</v>
       </c>
       <c r="B4" s="3">
-        <v>0.43472222222222223</v>
+        <v>0.45277777777777778</v>
       </c>
       <c r="C4" s="1">
         <v>4</v>
@@ -925,22 +921,22 @@
         <v>25</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F4" s="1">
-        <v>5890</v>
+        <v>610</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H4" s="1">
-        <v>0</v>
+        <v>4700</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J4" s="1">
-        <v>0</v>
+        <v>640</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>29</v>
@@ -985,15 +981,15 @@
         <v>0</v>
       </c>
       <c r="Y4" s="1">
-        <v>5890</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5950</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>43997</v>
       </c>
       <c r="B5" s="3">
-        <v>0.43472222222222223</v>
+        <v>0.47708333333333336</v>
       </c>
       <c r="C5" s="1">
         <v>4</v>
@@ -1002,19 +998,19 @@
         <v>25</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F5" s="1">
-        <v>5890</v>
+        <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H5" s="1">
         <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J5" s="1">
         <v>0</v>
@@ -1062,15 +1058,15 @@
         <v>0</v>
       </c>
       <c r="Y5" s="1">
-        <v>5890</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>43997</v>
       </c>
       <c r="B6" s="3">
-        <v>0.45277777777777778</v>
+        <v>0.47847222222222224</v>
       </c>
       <c r="C6" s="1">
         <v>4</v>
@@ -1079,22 +1075,22 @@
         <v>25</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F6" s="1">
-        <v>610</v>
+        <v>6030</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H6" s="1">
-        <v>4700</v>
+        <v>0</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J6" s="1">
-        <v>640</v>
+        <v>0</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>29</v>
@@ -1139,15 +1135,15 @@
         <v>0</v>
       </c>
       <c r="Y6" s="1">
-        <v>5950</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+        <v>6030</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>43997</v>
       </c>
       <c r="B7" s="3">
-        <v>0.47708333333333336</v>
+        <v>0.49583333333333335</v>
       </c>
       <c r="C7" s="1">
         <v>4</v>
@@ -1159,19 +1155,19 @@
         <v>26</v>
       </c>
       <c r="F7" s="1">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H7" s="1">
-        <v>0</v>
+        <v>4510</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>28</v>
       </c>
       <c r="J7" s="1">
-        <v>0</v>
+        <v>630</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>29</v>
@@ -1216,15 +1212,15 @@
         <v>0</v>
       </c>
       <c r="Y7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5740</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>43997</v>
       </c>
       <c r="B8" s="3">
-        <v>0.47847222222222224</v>
+        <v>0.52152777777777781</v>
       </c>
       <c r="C8" s="1">
         <v>4</v>
@@ -1236,7 +1232,7 @@
         <v>30</v>
       </c>
       <c r="F8" s="1">
-        <v>6030</v>
+        <v>5840</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>29</v>
@@ -1293,15 +1289,15 @@
         <v>0</v>
       </c>
       <c r="Y8" s="1">
-        <v>6030</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5840</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <v>43997</v>
+        <v>44007</v>
       </c>
       <c r="B9" s="3">
-        <v>0.47847222222222224</v>
+        <v>0.45694444444444443</v>
       </c>
       <c r="C9" s="1">
         <v>4</v>
@@ -1310,22 +1306,22 @@
         <v>25</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="F9" s="1">
-        <v>6430</v>
+        <v>590</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H9" s="1">
-        <v>0</v>
+        <v>4510</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J9" s="1">
-        <v>0</v>
+        <v>610</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>29</v>
@@ -1370,15 +1366,15 @@
         <v>0</v>
       </c>
       <c r="Y9" s="1">
-        <v>6030</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5710</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <v>43997</v>
+        <v>44007</v>
       </c>
       <c r="B10" s="3">
-        <v>0.49583333333333335</v>
+        <v>0.4777777777777778</v>
       </c>
       <c r="C10" s="1">
         <v>4</v>
@@ -1390,19 +1386,19 @@
         <v>26</v>
       </c>
       <c r="F10" s="1">
-        <v>600</v>
+        <v>10</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H10" s="1">
-        <v>4510</v>
+        <v>0</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>28</v>
       </c>
       <c r="J10" s="1">
-        <v>630</v>
+        <v>0</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>29</v>
@@ -1447,15 +1443,15 @@
         <v>0</v>
       </c>
       <c r="Y10" s="1">
-        <v>5740</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <v>43997</v>
+        <v>44007</v>
       </c>
       <c r="B11" s="3">
-        <v>0.52152777777777781</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="C11" s="1">
         <v>4</v>
@@ -1467,7 +1463,7 @@
         <v>30</v>
       </c>
       <c r="F11" s="1">
-        <v>5840</v>
+        <v>5730</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>29</v>
@@ -1524,15 +1520,15 @@
         <v>0</v>
       </c>
       <c r="Y11" s="1">
-        <v>5840</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5730</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>44007</v>
       </c>
       <c r="B12" s="3">
-        <v>0.45694444444444443</v>
+        <v>0.5</v>
       </c>
       <c r="C12" s="1">
         <v>4</v>
@@ -1550,13 +1546,13 @@
         <v>27</v>
       </c>
       <c r="H12" s="1">
-        <v>4510</v>
+        <v>4520</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>28</v>
       </c>
       <c r="J12" s="1">
-        <v>610</v>
+        <v>620</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>29</v>
@@ -1601,15 +1597,15 @@
         <v>0</v>
       </c>
       <c r="Y12" s="1">
-        <v>5710</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5730</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>44007</v>
       </c>
       <c r="B13" s="3">
-        <v>0.4777777777777778</v>
+        <v>0.57291666666666663</v>
       </c>
       <c r="C13" s="1">
         <v>4</v>
@@ -1681,12 +1677,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>44007</v>
       </c>
       <c r="B14" s="3">
-        <v>0.47916666666666669</v>
+        <v>0.57291666666666663</v>
       </c>
       <c r="C14" s="1">
         <v>4</v>
@@ -1698,7 +1694,7 @@
         <v>30</v>
       </c>
       <c r="F14" s="1">
-        <v>5730</v>
+        <v>5760</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>29</v>
@@ -1755,15 +1751,15 @@
         <v>0</v>
       </c>
       <c r="Y14" s="1">
-        <v>5730</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5760</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>44007</v>
       </c>
       <c r="B15" s="3">
-        <v>0.5</v>
+        <v>0.59513888888888888</v>
       </c>
       <c r="C15" s="1">
         <v>4</v>
@@ -1775,19 +1771,19 @@
         <v>26</v>
       </c>
       <c r="F15" s="1">
-        <v>590</v>
+        <v>0</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H15" s="1">
-        <v>4520</v>
+        <v>0</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>28</v>
       </c>
       <c r="J15" s="1">
-        <v>620</v>
+        <v>0</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>29</v>
@@ -1832,15 +1828,15 @@
         <v>0</v>
       </c>
       <c r="Y15" s="1">
-        <v>5730</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>44007</v>
       </c>
       <c r="B16" s="3">
-        <v>0.57291666666666663</v>
+        <v>0.59513888888888888</v>
       </c>
       <c r="C16" s="1">
         <v>4</v>
@@ -1852,7 +1848,7 @@
         <v>26</v>
       </c>
       <c r="F16" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>27</v>
@@ -1909,15 +1905,15 @@
         <v>0</v>
       </c>
       <c r="Y16" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>44007</v>
       </c>
       <c r="B17" s="3">
-        <v>0.57291666666666663</v>
+        <v>0.59583333333333333</v>
       </c>
       <c r="C17" s="1">
         <v>4</v>
@@ -1926,22 +1922,22 @@
         <v>25</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F17" s="1">
-        <v>5760</v>
+        <v>600</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H17" s="1">
-        <v>0</v>
+        <v>4560</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J17" s="1">
-        <v>0</v>
+        <v>630</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>29</v>
@@ -1986,15 +1982,15 @@
         <v>0</v>
       </c>
       <c r="Y17" s="1">
-        <v>5760</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5790</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>44007</v>
       </c>
       <c r="B18" s="3">
-        <v>0.57291666666666663</v>
+        <v>0.61736111111111114</v>
       </c>
       <c r="C18" s="1">
         <v>4</v>
@@ -2006,7 +2002,7 @@
         <v>30</v>
       </c>
       <c r="F18" s="1">
-        <v>5760</v>
+        <v>5670</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>29</v>
@@ -2063,15 +2059,15 @@
         <v>0</v>
       </c>
       <c r="Y18" s="1">
-        <v>5760</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5670</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
-        <v>44007</v>
+        <v>44014</v>
       </c>
       <c r="B19" s="3">
-        <v>0.59513888888888888</v>
+        <v>0.63541666666666663</v>
       </c>
       <c r="C19" s="1">
         <v>4</v>
@@ -2083,19 +2079,19 @@
         <v>26</v>
       </c>
       <c r="F19" s="1">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H19" s="1">
-        <v>0</v>
+        <v>4500</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>28</v>
       </c>
       <c r="J19" s="1">
-        <v>0</v>
+        <v>610</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>29</v>
@@ -2140,15 +2136,15 @@
         <v>0</v>
       </c>
       <c r="Y19" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5710</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
-        <v>44007</v>
+        <v>44014</v>
       </c>
       <c r="B20" s="3">
-        <v>0.59513888888888888</v>
+        <v>0.66597222222222219</v>
       </c>
       <c r="C20" s="1">
         <v>4</v>
@@ -2157,19 +2153,19 @@
         <v>25</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F20" s="1">
-        <v>0</v>
+        <v>5740</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H20" s="1">
         <v>0</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J20" s="1">
         <v>0</v>
@@ -2217,15 +2213,15 @@
         <v>0</v>
       </c>
       <c r="Y20" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5740</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
-        <v>44007</v>
+        <v>44014</v>
       </c>
       <c r="B21" s="3">
-        <v>0.59583333333333333</v>
+        <v>0.68680555555555556</v>
       </c>
       <c r="C21" s="1">
         <v>4</v>
@@ -2243,13 +2239,13 @@
         <v>27</v>
       </c>
       <c r="H21" s="1">
-        <v>4560</v>
+        <v>4540</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>28</v>
       </c>
       <c r="J21" s="1">
-        <v>630</v>
+        <v>610</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>29</v>
@@ -2294,15 +2290,15 @@
         <v>0</v>
       </c>
       <c r="Y21" s="1">
-        <v>5790</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5750</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
-        <v>44007</v>
+        <v>44014</v>
       </c>
       <c r="B22" s="3">
-        <v>0.61736111111111114</v>
+        <v>0.70763888888888893</v>
       </c>
       <c r="C22" s="1">
         <v>4</v>
@@ -2314,7 +2310,7 @@
         <v>30</v>
       </c>
       <c r="F22" s="1">
-        <v>5670</v>
+        <v>5740</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>29</v>
@@ -2371,15 +2367,15 @@
         <v>0</v>
       </c>
       <c r="Y22" s="1">
-        <v>5670</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5740</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
-        <v>44014</v>
+        <v>44020</v>
       </c>
       <c r="B23" s="3">
-        <v>0.63541666666666663</v>
+        <v>0.46180555555555558</v>
       </c>
       <c r="C23" s="1">
         <v>4</v>
@@ -2397,13 +2393,13 @@
         <v>27</v>
       </c>
       <c r="H23" s="1">
-        <v>4500</v>
+        <v>4530</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>28</v>
       </c>
       <c r="J23" s="1">
-        <v>610</v>
+        <v>620</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>29</v>
@@ -2448,15 +2444,15 @@
         <v>0</v>
       </c>
       <c r="Y23" s="1">
-        <v>5710</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5750</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
-        <v>44014</v>
+        <v>44020</v>
       </c>
       <c r="B24" s="3">
-        <v>0.66597222222222219</v>
+        <v>0.48402777777777778</v>
       </c>
       <c r="C24" s="1">
         <v>4</v>
@@ -2468,7 +2464,7 @@
         <v>30</v>
       </c>
       <c r="F24" s="1">
-        <v>5740</v>
+        <v>5730</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>29</v>
@@ -2525,15 +2521,15 @@
         <v>0</v>
       </c>
       <c r="Y24" s="1">
-        <v>5740</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5730</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
-        <v>44014</v>
+        <v>44020</v>
       </c>
       <c r="B25" s="3">
-        <v>0.68680555555555556</v>
+        <v>0.50347222222222221</v>
       </c>
       <c r="C25" s="1">
         <v>4</v>
@@ -2545,19 +2541,19 @@
         <v>26</v>
       </c>
       <c r="F25" s="1">
-        <v>600</v>
+        <v>580</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H25" s="1">
-        <v>4540</v>
+        <v>4530</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>28</v>
       </c>
       <c r="J25" s="1">
-        <v>610</v>
+        <v>620</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>29</v>
@@ -2602,15 +2598,15 @@
         <v>0</v>
       </c>
       <c r="Y25" s="1">
-        <v>5750</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5730</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
-        <v>44014</v>
+        <v>44020</v>
       </c>
       <c r="B26" s="3">
-        <v>0.70763888888888893</v>
+        <v>0.5229166666666667</v>
       </c>
       <c r="C26" s="1">
         <v>4</v>
@@ -2622,7 +2618,7 @@
         <v>30</v>
       </c>
       <c r="F26" s="1">
-        <v>5740</v>
+        <v>5770</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>29</v>
@@ -2679,15 +2675,15 @@
         <v>0</v>
       </c>
       <c r="Y26" s="1">
-        <v>5740</v>
-      </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5770</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>44020</v>
       </c>
       <c r="B27" s="3">
-        <v>0.46180555555555558</v>
+        <v>0.54027777777777775</v>
       </c>
       <c r="C27" s="1">
         <v>4</v>
@@ -2699,19 +2695,19 @@
         <v>26</v>
       </c>
       <c r="F27" s="1">
-        <v>600</v>
+        <v>590</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H27" s="1">
-        <v>4530</v>
+        <v>4540</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>28</v>
       </c>
       <c r="J27" s="1">
-        <v>620</v>
+        <v>610</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>29</v>
@@ -2756,15 +2752,15 @@
         <v>0</v>
       </c>
       <c r="Y27" s="1">
-        <v>5750</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5740</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>44020</v>
       </c>
       <c r="B28" s="3">
-        <v>0.48402777777777778</v>
+        <v>0.55902777777777779</v>
       </c>
       <c r="C28" s="1">
         <v>4</v>
@@ -2776,72 +2772,72 @@
         <v>30</v>
       </c>
       <c r="F28" s="1">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J28" s="1">
+        <v>0</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L28" s="1">
+        <v>0</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N28" s="1">
+        <v>0</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P28" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R28" s="1">
+        <v>0</v>
+      </c>
+      <c r="S28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T28" s="1">
+        <v>0</v>
+      </c>
+      <c r="U28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V28" s="1">
+        <v>0</v>
+      </c>
+      <c r="W28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="X28" s="1">
         <v>5730</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H28" s="1">
-        <v>0</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J28" s="1">
-        <v>0</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L28" s="1">
-        <v>0</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N28" s="1">
-        <v>0</v>
-      </c>
-      <c r="O28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P28" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="R28" s="1">
-        <v>0</v>
-      </c>
-      <c r="S28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T28" s="1">
-        <v>0</v>
-      </c>
-      <c r="U28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="V28" s="1">
-        <v>0</v>
-      </c>
-      <c r="W28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="X28" s="1">
-        <v>0</v>
       </c>
       <c r="Y28" s="1">
         <v>5730</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
-        <v>44020</v>
+        <v>44027</v>
       </c>
       <c r="B29" s="3">
-        <v>0.50347222222222221</v>
+        <v>0.43472222222222223</v>
       </c>
       <c r="C29" s="1">
         <v>4</v>
@@ -2853,7 +2849,7 @@
         <v>26</v>
       </c>
       <c r="F29" s="1">
-        <v>580</v>
+        <v>610</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>27</v>
@@ -2865,7 +2861,7 @@
         <v>28</v>
       </c>
       <c r="J29" s="1">
-        <v>620</v>
+        <v>600</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>29</v>
@@ -2910,15 +2906,15 @@
         <v>0</v>
       </c>
       <c r="Y29" s="1">
-        <v>5730</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5740</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
-        <v>44020</v>
+        <v>44027</v>
       </c>
       <c r="B30" s="3">
-        <v>0.5229166666666667</v>
+        <v>0.4597222222222222</v>
       </c>
       <c r="C30" s="1">
         <v>4</v>
@@ -2930,7 +2926,7 @@
         <v>30</v>
       </c>
       <c r="F30" s="1">
-        <v>5770</v>
+        <v>5750</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>29</v>
@@ -2987,15 +2983,15 @@
         <v>0</v>
       </c>
       <c r="Y30" s="1">
-        <v>5770</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5750</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
-        <v>44020</v>
+        <v>44027</v>
       </c>
       <c r="B31" s="3">
-        <v>0.54027777777777775</v>
+        <v>0.50069444444444444</v>
       </c>
       <c r="C31" s="1">
         <v>4</v>
@@ -3007,13 +3003,13 @@
         <v>26</v>
       </c>
       <c r="F31" s="1">
-        <v>590</v>
+        <v>610</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H31" s="1">
-        <v>4540</v>
+        <v>4520</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>28</v>
@@ -3067,12 +3063,12 @@
         <v>5740</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
-        <v>44020</v>
+        <v>44027</v>
       </c>
       <c r="B32" s="3">
-        <v>0.55902777777777779</v>
+        <v>0.60833333333333328</v>
       </c>
       <c r="C32" s="1">
         <v>4</v>
@@ -3084,72 +3080,72 @@
         <v>30</v>
       </c>
       <c r="F32" s="1">
-        <v>0</v>
+        <v>5670</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H32" s="1">
         <v>0</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J32" s="1">
         <v>0</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="L32" s="1">
         <v>0</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="N32" s="1">
         <v>0</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="P32" s="1">
         <v>0</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="R32" s="1">
         <v>0</v>
       </c>
       <c r="S32" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="T32" s="1">
         <v>0</v>
       </c>
       <c r="U32" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="V32" s="1">
         <v>0</v>
       </c>
       <c r="W32" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="X32" s="1">
-        <v>5730</v>
+        <v>0</v>
       </c>
       <c r="Y32" s="1">
-        <v>5730</v>
-      </c>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5670</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>44027</v>
       </c>
       <c r="B33" s="3">
-        <v>0.43472222222222223</v>
+        <v>0.67569444444444449</v>
       </c>
       <c r="C33" s="1">
         <v>4</v>
@@ -3161,19 +3157,19 @@
         <v>26</v>
       </c>
       <c r="F33" s="1">
-        <v>610</v>
+        <v>630</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H33" s="1">
-        <v>4530</v>
+        <v>4510</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>28</v>
       </c>
       <c r="J33" s="1">
-        <v>600</v>
+        <v>620</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>29</v>
@@ -3218,15 +3214,15 @@
         <v>0</v>
       </c>
       <c r="Y33" s="1">
-        <v>5740</v>
-      </c>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5760</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>44027</v>
       </c>
       <c r="B34" s="3">
-        <v>0.4597222222222222</v>
+        <v>0.71250000000000002</v>
       </c>
       <c r="C34" s="1">
         <v>4</v>
@@ -3298,12 +3294,12 @@
         <v>5750</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
-        <v>44027</v>
+        <v>44034</v>
       </c>
       <c r="B35" s="3">
-        <v>0.50069444444444444</v>
+        <v>0.48958333333333331</v>
       </c>
       <c r="C35" s="1">
         <v>4</v>
@@ -3315,19 +3311,19 @@
         <v>26</v>
       </c>
       <c r="F35" s="1">
-        <v>610</v>
+        <v>90</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H35" s="1">
-        <v>4520</v>
+        <v>0</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>28</v>
       </c>
       <c r="J35" s="1">
-        <v>610</v>
+        <v>0</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>29</v>
@@ -3372,15 +3368,15 @@
         <v>0</v>
       </c>
       <c r="Y35" s="1">
-        <v>5740</v>
-      </c>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
-        <v>44027</v>
+        <v>44034</v>
       </c>
       <c r="B36" s="3">
-        <v>0.60833333333333328</v>
+        <v>0.4909722222222222</v>
       </c>
       <c r="C36" s="1">
         <v>4</v>
@@ -3389,22 +3385,22 @@
         <v>25</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F36" s="1">
-        <v>5670</v>
+        <v>600</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H36" s="1">
-        <v>0</v>
+        <v>4580</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J36" s="1">
-        <v>0</v>
+        <v>660</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>29</v>
@@ -3449,15 +3445,15 @@
         <v>0</v>
       </c>
       <c r="Y36" s="1">
-        <v>5670</v>
-      </c>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5840</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
-        <v>44027</v>
+        <v>44034</v>
       </c>
       <c r="B37" s="3">
-        <v>0.67569444444444449</v>
+        <v>0.61388888888888893</v>
       </c>
       <c r="C37" s="1">
         <v>4</v>
@@ -3469,19 +3465,19 @@
         <v>26</v>
       </c>
       <c r="F37" s="1">
-        <v>630</v>
+        <v>0</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H37" s="1">
-        <v>4510</v>
+        <v>0</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>28</v>
       </c>
       <c r="J37" s="1">
-        <v>620</v>
+        <v>0</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>29</v>
@@ -3526,15 +3522,15 @@
         <v>0</v>
       </c>
       <c r="Y37" s="1">
-        <v>5760</v>
-      </c>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
-        <v>44027</v>
+        <v>44034</v>
       </c>
       <c r="B38" s="3">
-        <v>0.71250000000000002</v>
+        <v>0.61527777777777781</v>
       </c>
       <c r="C38" s="1">
         <v>4</v>
@@ -3546,7 +3542,7 @@
         <v>30</v>
       </c>
       <c r="F38" s="1">
-        <v>5750</v>
+        <v>5820</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>29</v>
@@ -3603,15 +3599,15 @@
         <v>0</v>
       </c>
       <c r="Y38" s="1">
-        <v>5750</v>
-      </c>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5820</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>44034</v>
       </c>
       <c r="B39" s="3">
-        <v>0.48958333333333331</v>
+        <v>0.65486111111111112</v>
       </c>
       <c r="C39" s="1">
         <v>4</v>
@@ -3623,19 +3619,19 @@
         <v>26</v>
       </c>
       <c r="F39" s="1">
-        <v>90</v>
+        <v>620</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H39" s="1">
-        <v>0</v>
+        <v>4520</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>28</v>
       </c>
       <c r="J39" s="1">
-        <v>0</v>
+        <v>610</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>29</v>
@@ -3680,15 +3676,15 @@
         <v>0</v>
       </c>
       <c r="Y39" s="1">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5750</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>44034</v>
       </c>
       <c r="B40" s="3">
-        <v>0.4909722222222222</v>
+        <v>0.67708333333333337</v>
       </c>
       <c r="C40" s="1">
         <v>4</v>
@@ -3697,22 +3693,22 @@
         <v>25</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F40" s="1">
-        <v>600</v>
+        <v>5750</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H40" s="1">
-        <v>4580</v>
+        <v>0</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J40" s="1">
-        <v>660</v>
+        <v>0</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>29</v>
@@ -3757,15 +3753,15 @@
         <v>0</v>
       </c>
       <c r="Y40" s="1">
-        <v>5840</v>
-      </c>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5750</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>44034</v>
       </c>
       <c r="B41" s="3">
-        <v>0.61388888888888893</v>
+        <v>0.70277777777777772</v>
       </c>
       <c r="C41" s="1">
         <v>4</v>
@@ -3777,19 +3773,19 @@
         <v>26</v>
       </c>
       <c r="F41" s="1">
-        <v>0</v>
+        <v>620</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H41" s="1">
-        <v>0</v>
+        <v>4520</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>28</v>
       </c>
       <c r="J41" s="1">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="K41" s="1" t="s">
         <v>29</v>
@@ -3834,15 +3830,15 @@
         <v>0</v>
       </c>
       <c r="Y41" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5740</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>44034</v>
       </c>
       <c r="B42" s="3">
-        <v>0.61527777777777781</v>
+        <v>0.72152777777777777</v>
       </c>
       <c r="C42" s="1">
         <v>4</v>
@@ -3854,7 +3850,7 @@
         <v>30</v>
       </c>
       <c r="F42" s="1">
-        <v>5820</v>
+        <v>5590</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>29</v>
@@ -3911,15 +3907,15 @@
         <v>0</v>
       </c>
       <c r="Y42" s="1">
-        <v>5820</v>
-      </c>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5590</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
-        <v>44034</v>
+        <v>44041</v>
       </c>
       <c r="B43" s="3">
-        <v>0.65486111111111112</v>
+        <v>0.48680555555555555</v>
       </c>
       <c r="C43" s="1">
         <v>4</v>
@@ -3937,7 +3933,7 @@
         <v>27</v>
       </c>
       <c r="H43" s="1">
-        <v>4520</v>
+        <v>4500</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>28</v>
@@ -3988,15 +3984,15 @@
         <v>0</v>
       </c>
       <c r="Y43" s="1">
-        <v>5750</v>
-      </c>
-    </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5730</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
-        <v>44034</v>
+        <v>44041</v>
       </c>
       <c r="B44" s="3">
-        <v>0.67708333333333337</v>
+        <v>0.61597222222222225</v>
       </c>
       <c r="C44" s="1">
         <v>4</v>
@@ -4008,7 +4004,7 @@
         <v>30</v>
       </c>
       <c r="F44" s="1">
-        <v>5750</v>
+        <v>5680</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>29</v>
@@ -4065,15 +4061,15 @@
         <v>0</v>
       </c>
       <c r="Y44" s="1">
-        <v>5750</v>
-      </c>
-    </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5680</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
-        <v>44034</v>
+        <v>44041</v>
       </c>
       <c r="B45" s="3">
-        <v>0.70277777777777772</v>
+        <v>0.64375000000000004</v>
       </c>
       <c r="C45" s="1">
         <v>4</v>
@@ -4085,13 +4081,13 @@
         <v>26</v>
       </c>
       <c r="F45" s="1">
-        <v>620</v>
+        <v>640</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H45" s="1">
-        <v>4520</v>
+        <v>4510</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>28</v>
@@ -4142,15 +4138,15 @@
         <v>0</v>
       </c>
       <c r="Y45" s="1">
-        <v>5740</v>
-      </c>
-    </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5750</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
-        <v>44034</v>
+        <v>44041</v>
       </c>
       <c r="B46" s="3">
-        <v>0.72152777777777777</v>
+        <v>0.66736111111111107</v>
       </c>
       <c r="C46" s="1">
         <v>4</v>
@@ -4162,7 +4158,7 @@
         <v>30</v>
       </c>
       <c r="F46" s="1">
-        <v>5590</v>
+        <v>5690</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>29</v>
@@ -4219,15 +4215,15 @@
         <v>0</v>
       </c>
       <c r="Y46" s="1">
-        <v>5590</v>
-      </c>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5690</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>44041</v>
       </c>
       <c r="B47" s="3">
-        <v>0.48680555555555555</v>
+        <v>0.7</v>
       </c>
       <c r="C47" s="1">
         <v>4</v>
@@ -4239,19 +4235,19 @@
         <v>26</v>
       </c>
       <c r="F47" s="1">
-        <v>620</v>
+        <v>600</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H47" s="1">
-        <v>4500</v>
+        <v>4520</v>
       </c>
       <c r="I47" s="1" t="s">
         <v>28</v>
       </c>
       <c r="J47" s="1">
-        <v>610</v>
+        <v>600</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>29</v>
@@ -4296,15 +4292,15 @@
         <v>0</v>
       </c>
       <c r="Y47" s="1">
-        <v>5730</v>
-      </c>
-    </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5720</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>44041</v>
       </c>
       <c r="B48" s="3">
-        <v>0.61597222222222225</v>
+        <v>0.71875</v>
       </c>
       <c r="C48" s="1">
         <v>4</v>
@@ -4316,7 +4312,7 @@
         <v>30</v>
       </c>
       <c r="F48" s="1">
-        <v>5680</v>
+        <v>5690</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>29</v>
@@ -4373,45 +4369,45 @@
         <v>0</v>
       </c>
       <c r="Y48" s="1">
-        <v>5680</v>
-      </c>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
+        <v>5690</v>
+      </c>
+    </row>
+    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
-        <v>44041</v>
+        <v>44103</v>
       </c>
       <c r="B49" s="3">
-        <v>0.64375000000000004</v>
+        <v>0.73124999999999996</v>
       </c>
       <c r="C49" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F49" s="1">
-        <v>640</v>
+        <v>610</v>
       </c>
       <c r="G49" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H49" s="1">
+        <v>250</v>
+      </c>
+      <c r="I49" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H49" s="1">
-        <v>4510</v>
-      </c>
-      <c r="I49" s="1" t="s">
+      <c r="J49" s="1">
+        <v>4630</v>
+      </c>
+      <c r="K49" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J49" s="1">
-        <v>600</v>
-      </c>
-      <c r="K49" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="L49" s="1">
-        <v>0</v>
+        <v>610</v>
       </c>
       <c r="M49" s="1" t="s">
         <v>29</v>
@@ -4450,39 +4446,39 @@
         <v>0</v>
       </c>
       <c r="Y49" s="1">
-        <v>5750</v>
-      </c>
-    </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
+        <v>6100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
-        <v>44041</v>
+        <v>44103</v>
       </c>
       <c r="B50" s="3">
-        <v>0.66736111111111107</v>
+        <v>0.76597222222222228</v>
       </c>
       <c r="C50" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F50" s="1">
-        <v>5690</v>
+        <v>50</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="H50" s="1">
-        <v>0</v>
+        <v>5890</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="J50" s="1">
-        <v>0</v>
+        <v>5870</v>
       </c>
       <c r="K50" s="1" t="s">
         <v>29</v>
@@ -4527,314 +4523,6 @@
         <v>0</v>
       </c>
       <c r="Y50" s="1">
-        <v>5690</v>
-      </c>
-    </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A51" s="2">
-        <v>44041</v>
-      </c>
-      <c r="B51" s="3">
-        <v>0.7</v>
-      </c>
-      <c r="C51" s="1">
-        <v>4</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F51" s="1">
-        <v>600</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H51" s="1">
-        <v>4520</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J51" s="1">
-        <v>600</v>
-      </c>
-      <c r="K51" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L51" s="1">
-        <v>0</v>
-      </c>
-      <c r="M51" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N51" s="1">
-        <v>0</v>
-      </c>
-      <c r="O51" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P51" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q51" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="R51" s="1">
-        <v>0</v>
-      </c>
-      <c r="S51" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T51" s="1">
-        <v>0</v>
-      </c>
-      <c r="U51" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="V51" s="1">
-        <v>0</v>
-      </c>
-      <c r="W51" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="X51" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y51" s="1">
-        <v>5720</v>
-      </c>
-    </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A52" s="2">
-        <v>44041</v>
-      </c>
-      <c r="B52" s="3">
-        <v>0.71875</v>
-      </c>
-      <c r="C52" s="1">
-        <v>4</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F52" s="1">
-        <v>5690</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H52" s="1">
-        <v>0</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J52" s="1">
-        <v>0</v>
-      </c>
-      <c r="K52" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L52" s="1">
-        <v>0</v>
-      </c>
-      <c r="M52" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N52" s="1">
-        <v>0</v>
-      </c>
-      <c r="O52" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P52" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q52" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="R52" s="1">
-        <v>0</v>
-      </c>
-      <c r="S52" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T52" s="1">
-        <v>0</v>
-      </c>
-      <c r="U52" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="V52" s="1">
-        <v>0</v>
-      </c>
-      <c r="W52" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="X52" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y52" s="1">
-        <v>5690</v>
-      </c>
-    </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A53" s="2">
-        <v>44103</v>
-      </c>
-      <c r="B53" s="3">
-        <v>0.73124999999999996</v>
-      </c>
-      <c r="C53" s="1">
-        <v>3</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F53" s="1">
-        <v>610</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H53" s="1">
-        <v>250</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J53" s="1">
-        <v>4630</v>
-      </c>
-      <c r="K53" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L53" s="1">
-        <v>610</v>
-      </c>
-      <c r="M53" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N53" s="1">
-        <v>0</v>
-      </c>
-      <c r="O53" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P53" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q53" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="R53" s="1">
-        <v>0</v>
-      </c>
-      <c r="S53" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T53" s="1">
-        <v>0</v>
-      </c>
-      <c r="U53" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="V53" s="1">
-        <v>0</v>
-      </c>
-      <c r="W53" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="X53" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y53" s="1">
-        <v>6100</v>
-      </c>
-    </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A54" s="2">
-        <v>44103</v>
-      </c>
-      <c r="B54" s="3">
-        <v>0.76597222222222228</v>
-      </c>
-      <c r="C54" s="1">
-        <v>3</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F54" s="1">
-        <v>50</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H54" s="1">
-        <v>5890</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J54" s="1">
-        <v>5870</v>
-      </c>
-      <c r="K54" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L54" s="1">
-        <v>0</v>
-      </c>
-      <c r="M54" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N54" s="1">
-        <v>0</v>
-      </c>
-      <c r="O54" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P54" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q54" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="R54" s="1">
-        <v>0</v>
-      </c>
-      <c r="S54" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T54" s="1">
-        <v>0</v>
-      </c>
-      <c r="U54" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="V54" s="1">
-        <v>0</v>
-      </c>
-      <c r="W54" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="X54" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y54" s="1">
         <v>1810</v>
       </c>
     </row>

</xml_diff>